<commit_message>
Added transaction lister and Portfolio maker.
</commit_message>
<xml_diff>
--- a/Crypto2.xlsx
+++ b/Crypto2.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2717500</v>
+        <v>2765308</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>121500</v>
+        <v>122500</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>32.25</v>
+        <v>32.355</v>
       </c>
     </row>
     <row r="5">

</xml_diff>